<commit_message>
Updated Oxidation Buffer Recipe
Added new sheet with slightly different solution recipe protocol
</commit_message>
<xml_diff>
--- a/Biochemistry/Hydroxyproline Assay/RecipeSheets/HydroxyprolineStandards_soln_recipes.xlsx
+++ b/Biochemistry/Hydroxyproline Assay/RecipeSheets/HydroxyprolineStandards_soln_recipes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atya222\Documents\GitHub\Protocols\Biochemistry\Hydroxyproline Assay\RecipeSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6820605D-5452-438A-AB79-5182DBA7976E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3A49E2-4E82-4187-A43F-0EF5DC597AAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -512,6 +512,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -524,7 +525,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -937,7 +940,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -955,10 +958,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1029,7 +1032,9 @@
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="E6" s="30">
+        <v>0.999</v>
+      </c>
       <c r="F6" s="19"/>
       <c r="G6" s="20" t="s">
         <v>13</v>
@@ -1054,10 +1059,10 @@
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="26"/>
+      <c r="B8" s="27"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -1072,7 +1077,7 @@
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="12" t="s">
         <v>2</v>
       </c>
@@ -1087,7 +1092,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="28" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="16" t="s">
@@ -1102,7 +1107,7 @@
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="18" t="s">
         <v>22</v>
       </c>
@@ -1113,7 +1118,7 @@
       <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="28" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="16" t="s">
@@ -1128,7 +1133,7 @@
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="18" t="s">
         <v>22</v>
       </c>
@@ -1139,7 +1144,7 @@
       <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="28" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="16" t="s">
@@ -1154,7 +1159,7 @@
       <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="18" t="s">
         <v>22</v>
       </c>
@@ -1165,7 +1170,7 @@
       <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="28" t="s">
         <v>35</v>
       </c>
       <c r="B18" s="16" t="s">
@@ -1180,7 +1185,7 @@
       <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="18" t="s">
         <v>22</v>
       </c>
@@ -1191,7 +1196,7 @@
       <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="28" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -1206,7 +1211,7 @@
       <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="18" t="s">
         <v>22</v>
       </c>
@@ -1217,7 +1222,7 @@
       <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="28" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="16" t="s">
@@ -1232,7 +1237,7 @@
       <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="18" t="s">
         <v>22</v>
       </c>
@@ -1243,7 +1248,7 @@
       <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
+      <c r="A24" s="28" t="s">
         <v>38</v>
       </c>
       <c r="B24" s="16" t="s">
@@ -1258,7 +1263,7 @@
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="18" t="s">
         <v>22</v>
       </c>
@@ -1269,7 +1274,7 @@
       <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="28" t="s">
         <v>39</v>
       </c>
       <c r="B26" s="16" t="s">
@@ -1284,7 +1289,7 @@
       <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="18" t="s">
         <v>22</v>
       </c>
@@ -1314,6 +1319,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100965EA08FA511AE4C9FFF632E6536ED13" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="abfa450e2c882fa05ec7f6a4b4016779">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a" xmlns:ns3="6cbc0c5a-d948-46e5-8624-1bad210f77c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53678093842f3275b6926b32e7a9c141" ns2:_="" ns3:_="">
     <xsd:import namespace="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
@@ -1536,22 +1556,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33AFEA7C-ECB0-4A51-9E17-02E120CDEEE9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
+    <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C3833AD-3BAD-44F9-A428-5312EFC8FF4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A161E6A-5B3F-4912-ADEE-71AD0FF6FC00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1568,29 +1598,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C3833AD-3BAD-44F9-A428-5312EFC8FF4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33AFEA7C-ECB0-4A51-9E17-02E120CDEEE9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6cbc0c5a-d948-46e5-8624-1bad210f77c7"/>
-    <ds:schemaRef ds:uri="5d5a2885-0f9b-4d04-9bc1-f867a2376b8a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>